<commit_message>
Fix transport workbook XML integrity
Co-authored-by: skuskuM <skuskuM@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/proiect/Proiect_Informatica_Transport.xlsx
+++ b/proiect/Proiect_Informatica_Transport.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ns1="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns2="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:ns3="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:ns4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:ns5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:ns6="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:ns7="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ns8="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:ns9="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" ns1:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
-  <ns1:AlternateContent>
-    <ns1:Choice Requires="x15">
-      <ns2:absPath url="/Users/tudormoldovan/Desktop/Proiect INFO/"/>
-    </ns1:Choice>
-  </ns1:AlternateContent>
-  <ns3:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB6EE26-578C-EF43-A888-6A9842CF09BF}" ns4:coauthVersionLast="45" ns4:coauthVersionMax="45" ns5:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudormoldovan/Desktop/Proiect INFO/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB6EE26-578C-EF43-A888-6A9842CF09BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" ns6:uid="{6A44DA51-D805-4D4E-AC6C-01D8CB486623}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{6A44DA51-D805-4D4E-AC6C-01D8CB486623}"/>
   </bookViews>
   <workbookProtection lockStructure="1"/>
   <sheets>
-    <sheet name="Acasa" sheetId="1" ns7:id="rId1"/>
-    <sheet name="Vehicule" sheetId="8" ns7:id="rId2"/>
-    <sheet name="Parc_Auto" sheetId="4" ns7:id="rId3"/>
-    <sheet name="Curse_S1" sheetId="9" ns7:id="rId4"/>
-    <sheet name="Raport_S1" sheetId="17" ns7:id="rId5"/>
-    <sheet name="Clienti_Fideli" sheetId="5" ns7:id="rId6"/>
-    <sheet name="Clienti_Curenti" sheetId="7" ns7:id="rId7"/>
-    <sheet name="Angajati" sheetId="6" ns7:id="rId8"/>
+    <sheet name="Acasa" sheetId="1" r:id="rId1"/>
+    <sheet name="Vehicule" sheetId="8" r:id="rId2"/>
+    <sheet name="Parc_Auto" sheetId="4" r:id="rId3"/>
+    <sheet name="Curse_S1" sheetId="9" r:id="rId4"/>
+    <sheet name="Raport_S1" sheetId="17" r:id="rId5"/>
+    <sheet name="Clienti_Fideli" sheetId="5" r:id="rId6"/>
+    <sheet name="Clienti_Curenti" sheetId="7" r:id="rId7"/>
+    <sheet name="Angajati" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="ACCES_DIR._CĂTRE_PISCINĂ">Vehicule!$K$4:$K$54</definedName>
-    <definedName name="Cameră_Delux">Vehicule!$D$16:$N$26</definedName>
-    <definedName name="Cameră_Palais">Vehicule!$D$27:$N$37</definedName>
-    <definedName name="Cameră_Superioară">Vehicule!$D$5:$N$15</definedName>
+    <definedName name="Duba">Vehicule!$D$16:$N$26</definedName>
+    <definedName name="Autocar">Vehicule!$D$27:$N$37</definedName>
+    <definedName name="Camion">Vehicule!$D$5:$N$15</definedName>
     <definedName name="Data_achizitiei">Parc_Auto!$M$4:$M$18</definedName>
     <definedName name="DATA_ELIBERĂRII">Vehicule!$N$4:$N$53</definedName>
     <definedName name="DATA_OCUPĂRII">Vehicule!$M$4:$M$54</definedName>
-    <definedName name="ETAJ">Vehicule!$J$4:$J$54</definedName>
+    <definedName name="AXE">Vehicule!$J$4:$J$54</definedName>
     <definedName name="Kilometraj">Parc_Auto!$L$4:$L$18</definedName>
     <definedName name="Marca">Parc_Auto!$D$4:$D$18</definedName>
     <definedName name="Model">Parc_Auto!$E$4:$E$18</definedName>
     <definedName name="Nr._locuri_pasageri">Parc_Auto!$N$4:$N$18</definedName>
-    <definedName name="Număr_cameră">Vehicule!$E$4:$E$54</definedName>
+    <definedName name="Numar_vehicul">Vehicule!$E$4:$E$54</definedName>
     <definedName name="Număr_de_înmatriculare">Parc_Auto!$I$4:$I$18</definedName>
     <definedName name="Nume">Clienti_Fideli!$D$4:$D$19</definedName>
     <definedName name="Nume_șofer">Parc_Auto!$O$4:$O$18</definedName>
@@ -44,35 +44,35 @@
     <definedName name="Prenume">Clienti_Fideli!$E$4:$E$19</definedName>
     <definedName name="PREȚ_NOAPTE">Vehicule!$I$4:$I$54</definedName>
     <definedName name="Serie_de_șasiu">Parc_Auto!$H$4:$H$18</definedName>
-    <definedName name="Suită_Delux">Vehicule!$D$43:$N$47</definedName>
-    <definedName name="Suită_Palais">Vehicule!$D$48:$N$52</definedName>
-    <definedName name="Suită_Sperioară">Vehicule!$D$38:$N$42</definedName>
+    <definedName name="Semiremorca">Vehicule!$D$43:$N$47</definedName>
+    <definedName name="Trailer">Vehicule!$D$48:$N$52</definedName>
+    <definedName name="Autoutilitara">Vehicule!$D$38:$N$42</definedName>
     <definedName name="SUPRAFAȚĂ_ÎN_m²">Vehicule!$F$4:$F$54</definedName>
-    <definedName name="TABEL_CAMERE">Vehicule!$D$4:$N$54</definedName>
+    <definedName name="TABEL_VEHICULE">Vehicule!$D$4:$N$54</definedName>
     <definedName name="Tip">Parc_Auto!$F$4:$F$18</definedName>
-    <definedName name="Tip_Cameră">Vehicule!$D$4:$D$54</definedName>
+    <definedName name="Tip_Vehicul">Vehicule!$D$4:$D$54</definedName>
     <definedName name="TIP_PAT">Vehicule!$G$4:$G$54</definedName>
     <definedName name="Ultima_revzie">Parc_Auto!$J$4:$J$18</definedName>
     <definedName name="Următoarea_revizie">Parc_Auto!$K$4:$K$18</definedName>
     <definedName name="Utilizare">Parc_Auto!$G$4:$G$18</definedName>
     <definedName name="VEDERE_LA_MARE">Vehicule!$H$4:$H$54</definedName>
-    <definedName name="Villa">Vehicule!$D$53:$N$54</definedName>
+    <definedName name="Platforma">Vehicule!$D$53:$N$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" ns7:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
   </pivotCaches>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <ns8:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <ns9:calcFeatures>
-        <ns9:feature name="microsoft.com:RD"/>
-        <ns9:feature name="microsoft.com:Single"/>
-        <ns9:feature name="microsoft.com:FV"/>
-        <ns9:feature name="microsoft.com:CNMTM"/>
-      </ns9:calcFeatures>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1032,13 +1032,13 @@
     <t>Sum of Total</t>
   </si>
   <si>
-    <t>Numar Vehicule</t>
+    <t>Număr Vehicule</t>
   </si>
   <si>
-    <t>Numar Vehicule Ocupate</t>
+    <t>Număr Vehicule Ocupate</t>
   </si>
   <si>
-    <t>Numar Vehicule Libere</t>
+    <t>Număr Vehicule Libere</t>
   </si>
   <si>
     <t>PRENUME</t>
@@ -5283,25 +5283,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5461,25 +5461,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5639,25 +5639,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5817,25 +5817,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5995,25 +5995,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6173,25 +6173,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Cameră Delux</c:v>
+                  <c:v>Duba</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cameră Palais</c:v>
+                  <c:v>Autocar</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cameră Superioară</c:v>
+                  <c:v>Camion</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Suită Delux</c:v>
+                  <c:v>Semiremorca</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Suită Palais</c:v>
+                  <c:v>Trailer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Suită Superioară</c:v>
+                  <c:v>Autoutilitara</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Villa</c:v>
+                  <c:v>Platforma</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9994,7 +9994,7 @@
               </a:solidFill>
               <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>CAMERE</a:t>
+            <a:t>VEHICULE</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -11144,13 +11144,13 @@
     </cacheField>
     <cacheField name="Tip cameră " numFmtId="0">
       <sharedItems count="7">
-        <s v="Cameră Superioară"/>
-        <s v="Cameră Delux"/>
-        <s v="Cameră Palais"/>
-        <s v="Suită Superioară"/>
-        <s v="Suită Delux"/>
-        <s v="Suită Palais"/>
-        <s v="Villa"/>
+        <s v="Camion"/>
+        <s v="Duba"/>
+        <s v="Autocar"/>
+        <s v="Autoutilitara"/>
+        <s v="Semiremorca"/>
+        <s v="Trailer"/>
+        <s v="Platforma"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Preț/Noapte" numFmtId="164">
@@ -11804,7 +11804,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89C5E35B-597E-8C43-BF46-21B0D30CA761}" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="TIP DE CAMERĂ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89C5E35B-597E-8C43-BF46-21B0D30CA761}" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="TIP VEHICUL">
   <location ref="D4:L12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="1" showAll="0"/>
@@ -12341,9 +12341,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{445B1395-C98D-AF48-A571-837111AFDE3E}" name="Table6" displayName="Table6" ref="D4:M54" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="D4:M54" xr:uid="{7F7E20C4-7D60-B44C-B7AE-94663AC865C1}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8460BB4F-C540-7644-BC97-A5543A1BCD67}" name="NUMĂR CAMERĂ" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{096AED7F-7211-614C-A5E9-3935BCCD9307}" name="TIP CAMERĂ "/>
-    <tableColumn id="3" xr3:uid="{343379CA-0150-0041-87E7-A878BE16311B}" name="PREȚ/NOAPTE" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{8460BB4F-C540-7644-BC97-A5543A1BCD67}" name="NUMAR VEHICUL" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{096AED7F-7211-614C-A5E9-3935BCCD9307}" name="TIP VEHICUL "/>
+    <tableColumn id="3" xr3:uid="{343379CA-0150-0041-87E7-A878BE16311B}" name="TARIF/KM" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(D5,Vehicule!E:Q,5,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{40B824F1-CE7E-2649-9648-054D21FA38F3}" name="IANUARIE"/>
@@ -12353,7 +12353,7 @@
     <tableColumn id="8" xr3:uid="{20050490-2E67-4E4C-BB7B-44DC91164229}" name="MAI"/>
     <tableColumn id="9" xr3:uid="{42BBB5E7-3130-4247-B0E5-41A2AD2DA12C}" name="IUNIE"/>
     <tableColumn id="10" xr3:uid="{DF1D7209-9106-E14F-8044-63D1B28DBBCF}" name="TOTAL" dataDxfId="8">
-      <calculatedColumnFormula>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>

</xml_diff>

<commit_message>
Rebuild transport workbook for Excel compatibility
Co-authored-by: skuskuM <skuskuM@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/proiect/Proiect_Informatica_Transport.xlsx
+++ b/proiect/Proiect_Informatica_Transport.xlsx
@@ -12,51 +12,50 @@
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{6A44DA51-D805-4D4E-AC6C-01D8CB486623}"/>
   </bookViews>
-  <workbookProtection lockStructure="1"/>
   <sheets>
-    <sheet name="Acasa" sheetId="1" r:id="rId1"/>
-    <sheet name="Vehicule" sheetId="8" r:id="rId2"/>
-    <sheet name="Parc_Auto" sheetId="4" r:id="rId3"/>
-    <sheet name="Curse_S1" sheetId="9" r:id="rId4"/>
-    <sheet name="Raport_S1" sheetId="17" r:id="rId5"/>
-    <sheet name="Clienti_Fideli" sheetId="5" r:id="rId6"/>
-    <sheet name="Clienti_Curenti" sheetId="7" r:id="rId7"/>
+    <sheet name="Acasă" sheetId="1" r:id="rId1"/>
+    <sheet name="Camere" sheetId="8" r:id="rId2"/>
+    <sheet name="Autovehicule Transport Aproviz" sheetId="4" r:id="rId3"/>
+    <sheet name="Nr nopți ocpt in prima jum an" sheetId="9" r:id="rId4"/>
+    <sheet name="PT Raport Prima Jum An " sheetId="17" r:id="rId5"/>
+    <sheet name="Clienti Fideli" sheetId="5" r:id="rId6"/>
+    <sheet name="Clienti actuali" sheetId="7" r:id="rId7"/>
     <sheet name="Angajati" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="ACCES_DIR._CĂTRE_PISCINĂ">Vehicule!$K$4:$K$54</definedName>
-    <definedName name="Duba">Vehicule!$D$16:$N$26</definedName>
-    <definedName name="Autocar">Vehicule!$D$27:$N$37</definedName>
-    <definedName name="Camion">Vehicule!$D$5:$N$15</definedName>
-    <definedName name="Data_achizitiei">Parc_Auto!$M$4:$M$18</definedName>
-    <definedName name="DATA_ELIBERĂRII">Vehicule!$N$4:$N$53</definedName>
-    <definedName name="DATA_OCUPĂRII">Vehicule!$M$4:$M$54</definedName>
-    <definedName name="AXE">Vehicule!$J$4:$J$54</definedName>
-    <definedName name="Kilometraj">Parc_Auto!$L$4:$L$18</definedName>
-    <definedName name="Marca">Parc_Auto!$D$4:$D$18</definedName>
-    <definedName name="Model">Parc_Auto!$E$4:$E$18</definedName>
-    <definedName name="Nr._locuri_pasageri">Parc_Auto!$N$4:$N$18</definedName>
-    <definedName name="Numar_vehicul">Vehicule!$E$4:$E$54</definedName>
-    <definedName name="Număr_de_înmatriculare">Parc_Auto!$I$4:$I$18</definedName>
-    <definedName name="Nume">Clienti_Fideli!$D$4:$D$19</definedName>
-    <definedName name="Nume_șofer">Parc_Auto!$O$4:$O$18</definedName>
-    <definedName name="OCUPATĂ_LIBERĂ">Vehicule!$L$4:$L$54</definedName>
-    <definedName name="Prenume">Clienti_Fideli!$E$4:$E$19</definedName>
-    <definedName name="PREȚ_NOAPTE">Vehicule!$I$4:$I$54</definedName>
-    <definedName name="Serie_de_șasiu">Parc_Auto!$H$4:$H$18</definedName>
-    <definedName name="Semiremorca">Vehicule!$D$43:$N$47</definedName>
-    <definedName name="Trailer">Vehicule!$D$48:$N$52</definedName>
-    <definedName name="Autoutilitara">Vehicule!$D$38:$N$42</definedName>
-    <definedName name="SUPRAFAȚĂ_ÎN_m²">Vehicule!$F$4:$F$54</definedName>
-    <definedName name="TABEL_VEHICULE">Vehicule!$D$4:$N$54</definedName>
-    <definedName name="Tip">Parc_Auto!$F$4:$F$18</definedName>
-    <definedName name="Tip_Vehicul">Vehicule!$D$4:$D$54</definedName>
-    <definedName name="TIP_PAT">Vehicule!$G$4:$G$54</definedName>
-    <definedName name="Ultima_revzie">Parc_Auto!$J$4:$J$18</definedName>
-    <definedName name="Următoarea_revizie">Parc_Auto!$K$4:$K$18</definedName>
-    <definedName name="Utilizare">Parc_Auto!$G$4:$G$18</definedName>
-    <definedName name="VEDERE_LA_MARE">Vehicule!$H$4:$H$54</definedName>
-    <definedName name="Platforma">Vehicule!$D$53:$N$54</definedName>
+    <definedName name="ACCES_DIR._CĂTRE_PISCINĂ">Camere!$K$4:$K$54</definedName>
+    <definedName name="Cameră_Delux">Camere!$D$16:$N$26</definedName>
+    <definedName name="Cameră_Palais">Camere!$D$27:$N$37</definedName>
+    <definedName name="Cameră_Superioară">Camere!$D$5:$N$15</definedName>
+    <definedName name="Data_achizitiei">'Autovehicule Transport Aproviz'!$M$4:$M$18</definedName>
+    <definedName name="DATA_ELIBERĂRII">Camere!$N$4:$N$53</definedName>
+    <definedName name="DATA_OCUPĂRII">Camere!$M$4:$M$54</definedName>
+    <definedName name="ETAJ">Camere!$J$4:$J$54</definedName>
+    <definedName name="Kilometraj">'Autovehicule Transport Aproviz'!$L$4:$L$18</definedName>
+    <definedName name="Marca">'Autovehicule Transport Aproviz'!$D$4:$D$18</definedName>
+    <definedName name="Model">'Autovehicule Transport Aproviz'!$E$4:$E$18</definedName>
+    <definedName name="Nr._locuri_pasageri">'Autovehicule Transport Aproviz'!$N$4:$N$18</definedName>
+    <definedName name="Număr_cameră">Camere!$E$4:$E$54</definedName>
+    <definedName name="Număr_de_înmatriculare">'Autovehicule Transport Aproviz'!$I$4:$I$18</definedName>
+    <definedName name="Nume">'Clienti Fideli'!$D$4:$D$19</definedName>
+    <definedName name="Nume_șofer">'Autovehicule Transport Aproviz'!$O$4:$O$18</definedName>
+    <definedName name="OCUPATĂ_LIBERĂ">Camere!$L$4:$L$54</definedName>
+    <definedName name="Prenume">'Clienti Fideli'!$E$4:$E$19</definedName>
+    <definedName name="PREȚ_NOAPTE">Camere!$I$4:$I$54</definedName>
+    <definedName name="Serie_de_șasiu">'Autovehicule Transport Aproviz'!$H$4:$H$18</definedName>
+    <definedName name="Suită_Delux">Camere!$D$43:$N$47</definedName>
+    <definedName name="Suită_Palais">Camere!$D$48:$N$52</definedName>
+    <definedName name="Suită_Sperioară">Camere!$D$38:$N$42</definedName>
+    <definedName name="SUPRAFAȚĂ_ÎN_m²">Camere!$F$4:$F$54</definedName>
+    <definedName name="TABEL_CAMERE">Camere!$D$4:$N$54</definedName>
+    <definedName name="Tip">'Autovehicule Transport Aproviz'!$F$4:$F$18</definedName>
+    <definedName name="Tip_Cameră">Camere!$D$4:$D$54</definedName>
+    <definedName name="TIP_PAT">Camere!$G$4:$G$54</definedName>
+    <definedName name="Ultima_revzie">'Autovehicule Transport Aproviz'!$J$4:$J$18</definedName>
+    <definedName name="Următoarea_revizie">'Autovehicule Transport Aproviz'!$K$4:$K$18</definedName>
+    <definedName name="Utilizare">'Autovehicule Transport Aproviz'!$G$4:$G$18</definedName>
+    <definedName name="VEDERE_LA_MARE">Camere!$H$4:$H$54</definedName>
+    <definedName name="Villa">Camere!$D$53:$N$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -1032,13 +1031,13 @@
     <t>Sum of Total</t>
   </si>
   <si>
-    <t>Număr Vehicule</t>
+    <t>Numar Vehicule</t>
   </si>
   <si>
-    <t>Număr Vehicule Ocupate</t>
+    <t>Numar Vehicule Ocupate</t>
   </si>
   <si>
-    <t>Număr Vehicule Libere</t>
+    <t>Numar Vehicule Libere</t>
   </si>
   <si>
     <t>PRENUME</t>
@@ -3886,21 +3885,21 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Vehicule!$S$4:$S$5</c:f>
+              <c:f>Camere!$S$4:$S$5</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Număr Vehicule Ocupate</c:v>
+                  <c:v>Numar Vehicule Ocupate</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Număr Vehicule Libere</c:v>
+                  <c:v>Numar Vehicule Libere</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Vehicule!$T$4:$T$5</c:f>
+              <c:f>Camere!$T$4:$T$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -4215,7 +4214,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>'Curse_S1'!$G$4:$K$4</c:f>
+              <c:f>'Nr nopți ocpt in prima jum an'!$G$4:$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4243,7 +4242,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Curse_S1'!$G$10:$K$10</c:f>
+              <c:f>'Nr nopți ocpt in prima jum an'!$G$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4287,7 +4286,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Curse_S1'!$F$4</c:f>
+              <c:f>'Nr nopți ocpt in prima jum an'!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4311,7 +4310,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Curse_S1'!$G$4:$K$4</c:f>
+              <c:f>'Nr nopți ocpt in prima jum an'!$G$4:$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4339,7 +4338,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Curse_S1'!$G$11:$K$11</c:f>
+              <c:f>'Nr nopți ocpt in prima jum an'!$G$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4581,7 +4580,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Grand-Hotel du Cote d'Azur.xlsx]Raport_S1!PivotTable1</c:name>
+    <c:name>[Grand-Hotel du Cote d'Azur.xlsx]PT Raport Prima Jum An !PivotTable1</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -5169,7 +5168,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BO$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BO$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5279,7 +5278,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5308,7 +5307,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BO$91:$BO$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BO$91:$BO$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5347,7 +5346,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BP$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BP$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5457,7 +5456,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5486,7 +5485,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BP$91:$BP$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BP$91:$BP$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5525,7 +5524,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BQ$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BQ$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5635,7 +5634,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5664,7 +5663,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BQ$91:$BQ$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BQ$91:$BQ$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5703,7 +5702,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BR$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BR$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5813,7 +5812,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5842,7 +5841,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BR$91:$BR$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BR$91:$BR$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5881,7 +5880,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BS$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BS$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5991,7 +5990,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -6020,7 +6019,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BS$91:$BS$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BS$91:$BS$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -6059,7 +6058,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Raport_S1!$BT$90</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BT$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6169,7 +6168,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Raport_S1!$BN$91:$BN$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BN$91:$BN$98</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -6198,7 +6197,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Raport_S1!$BT$91:$BT$98</c:f>
+              <c:f>'PT Raport Prima Jum An '!$BT$91:$BT$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -9994,7 +9993,7 @@
               </a:solidFill>
               <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>VEHICULE</a:t>
+            <a:t>CAMERE</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -11144,13 +11143,13 @@
     </cacheField>
     <cacheField name="Tip cameră " numFmtId="0">
       <sharedItems count="7">
-        <s v="Camion"/>
-        <s v="Duba"/>
-        <s v="Autocar"/>
-        <s v="Autoutilitara"/>
-        <s v="Semiremorca"/>
-        <s v="Trailer"/>
-        <s v="Platforma"/>
+        <s v="Cameră Superioară"/>
+        <s v="Cameră Delux"/>
+        <s v="Cameră Palais"/>
+        <s v="Suită Superioară"/>
+        <s v="Suită Delux"/>
+        <s v="Suită Palais"/>
+        <s v="Villa"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Preț/Noapte" numFmtId="164">
@@ -11804,7 +11803,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89C5E35B-597E-8C43-BF46-21B0D30CA761}" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="TIP VEHICUL">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{89C5E35B-597E-8C43-BF46-21B0D30CA761}" name="PivotTable7" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="TIP DE CAMERĂ">
   <location ref="D4:L12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField numFmtId="1" showAll="0"/>
@@ -12341,10 +12340,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{445B1395-C98D-AF48-A571-837111AFDE3E}" name="Table6" displayName="Table6" ref="D4:M54" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="D4:M54" xr:uid="{7F7E20C4-7D60-B44C-B7AE-94663AC865C1}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8460BB4F-C540-7644-BC97-A5543A1BCD67}" name="NUMAR VEHICUL" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{096AED7F-7211-614C-A5E9-3935BCCD9307}" name="TIP VEHICUL "/>
-    <tableColumn id="3" xr3:uid="{343379CA-0150-0041-87E7-A878BE16311B}" name="TARIF/KM" dataDxfId="9">
-      <calculatedColumnFormula>VLOOKUP(D5,Vehicule!E:Q,5,0)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{8460BB4F-C540-7644-BC97-A5543A1BCD67}" name="NUMĂR CAMERĂ" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{096AED7F-7211-614C-A5E9-3935BCCD9307}" name="TIP CAMERĂ "/>
+    <tableColumn id="3" xr3:uid="{343379CA-0150-0041-87E7-A878BE16311B}" name="PREȚ/NOAPTE" dataDxfId="9">
+      <calculatedColumnFormula>VLOOKUP(D5,Camere!E:Q,5,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{40B824F1-CE7E-2649-9648-054D21FA38F3}" name="IANUARIE"/>
     <tableColumn id="5" xr3:uid="{E8882B8E-9862-6349-991B-D03D96246599}" name="FEBRUARIE "/>
@@ -12353,7 +12352,7 @@
     <tableColumn id="8" xr3:uid="{20050490-2E67-4E4C-BB7B-44DC91164229}" name="MAI"/>
     <tableColumn id="9" xr3:uid="{42BBB5E7-3130-4247-B0E5-41A2AD2DA12C}" name="IUNIE"/>
     <tableColumn id="10" xr3:uid="{DF1D7209-9106-E14F-8044-63D1B28DBBCF}" name="TOTAL" dataDxfId="8">
-      <calculatedColumnFormula>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -23357,7 +23356,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="125">
-        <f>VLOOKUP(D5,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D5,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G5">
@@ -23379,7 +23378,7 @@
         <v>19</v>
       </c>
       <c r="M5" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>16905</v>
       </c>
       <c r="N5" s="4"/>
@@ -23441,7 +23440,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="125">
-        <f>VLOOKUP(D6,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D6,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G6">
@@ -23463,7 +23462,7 @@
         <v>21</v>
       </c>
       <c r="M6" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>16660</v>
       </c>
       <c r="N6" s="4"/>
@@ -23519,7 +23518,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="125">
-        <f>VLOOKUP(D7,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D7,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G7">
@@ -23541,7 +23540,7 @@
         <v>20</v>
       </c>
       <c r="M7" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>14455</v>
       </c>
       <c r="N7" s="4"/>
@@ -23585,7 +23584,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="125">
-        <f>VLOOKUP(D8,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D8,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G8">
@@ -23607,7 +23606,7 @@
         <v>19</v>
       </c>
       <c r="M8" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>15190</v>
       </c>
       <c r="N8" s="4"/>
@@ -23651,7 +23650,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="125">
-        <f>VLOOKUP(D9,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D9,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G9">
@@ -23673,7 +23672,7 @@
         <v>18</v>
       </c>
       <c r="M9" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>14210</v>
       </c>
       <c r="N9" s="4"/>
@@ -23717,7 +23716,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="125">
-        <f>VLOOKUP(D10,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D10,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G10">
@@ -23739,7 +23738,7 @@
         <v>19</v>
       </c>
       <c r="M10" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>15435</v>
       </c>
       <c r="N10" s="4"/>
@@ -23783,7 +23782,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="125">
-        <f>VLOOKUP(D11,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D11,Camere!E:Q,5,0)</f>
         <v>280</v>
       </c>
       <c r="G11">
@@ -23805,7 +23804,7 @@
         <v>17</v>
       </c>
       <c r="M11" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>17080</v>
       </c>
       <c r="N11" s="4"/>
@@ -23849,7 +23848,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="125">
-        <f>VLOOKUP(D12,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D12,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G12">
@@ -23871,7 +23870,7 @@
         <v>20</v>
       </c>
       <c r="M12" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>16905</v>
       </c>
       <c r="N12" s="4"/>
@@ -23915,7 +23914,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="125">
-        <f>VLOOKUP(D13,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D13,Camere!E:Q,5,0)</f>
         <v>280</v>
       </c>
       <c r="G13">
@@ -23937,7 +23936,7 @@
         <v>21</v>
       </c>
       <c r="M13" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>17640</v>
       </c>
       <c r="N13" s="4"/>
@@ -23981,7 +23980,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="125">
-        <f>VLOOKUP(D14,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D14,Camere!E:Q,5,0)</f>
         <v>245</v>
       </c>
       <c r="G14">
@@ -24003,7 +24002,7 @@
         <v>21</v>
       </c>
       <c r="M14" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>16415</v>
       </c>
       <c r="N14" s="4"/>
@@ -24047,7 +24046,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="125">
-        <f>VLOOKUP(D15,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D15,Camere!E:Q,5,0)</f>
         <v>280</v>
       </c>
       <c r="G15">
@@ -24069,7 +24068,7 @@
         <v>14</v>
       </c>
       <c r="M15" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>17080</v>
       </c>
       <c r="N15" s="4"/>
@@ -24113,7 +24112,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="127">
-        <f>VLOOKUP(D16,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D16,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G16">
@@ -24135,7 +24134,7 @@
         <v>13</v>
       </c>
       <c r="M16" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>28830</v>
       </c>
       <c r="N16" s="4"/>
@@ -24179,7 +24178,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="127">
-        <f>VLOOKUP(D17,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D17,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G17">
@@ -24201,7 +24200,7 @@
         <v>21</v>
       </c>
       <c r="M17" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>30690</v>
       </c>
       <c r="N17" s="4"/>
@@ -24245,7 +24244,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="127">
-        <f>VLOOKUP(D18,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D18,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G18">
@@ -24267,7 +24266,7 @@
         <v>12</v>
       </c>
       <c r="M18" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>26505</v>
       </c>
       <c r="N18" s="4"/>
@@ -24311,7 +24310,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="127">
-        <f>VLOOKUP(D19,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D19,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G19">
@@ -24333,7 +24332,7 @@
         <v>14</v>
       </c>
       <c r="M19" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>27900</v>
       </c>
       <c r="N19" s="4"/>
@@ -24377,7 +24376,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="127">
-        <f>VLOOKUP(D20,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D20,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G20">
@@ -24399,7 +24398,7 @@
         <v>21</v>
       </c>
       <c r="M20" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>31620</v>
       </c>
       <c r="N20" s="4"/>
@@ -24443,7 +24442,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="127">
-        <f>VLOOKUP(D21,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D21,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G21">
@@ -24465,7 +24464,7 @@
         <v>22</v>
       </c>
       <c r="M21" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>33945</v>
       </c>
       <c r="N21" s="4"/>
@@ -24509,7 +24508,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="127">
-        <f>VLOOKUP(D22,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D22,Camere!E:Q,5,0)</f>
         <v>500</v>
       </c>
       <c r="G22">
@@ -24531,7 +24530,7 @@
         <v>18</v>
       </c>
       <c r="M22" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>32500</v>
       </c>
       <c r="N22" s="4"/>
@@ -24575,7 +24574,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="127">
-        <f>VLOOKUP(D23,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D23,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G23">
@@ -24597,7 +24596,7 @@
         <v>18</v>
       </c>
       <c r="M23" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>30690</v>
       </c>
       <c r="N23" s="4"/>
@@ -24641,7 +24640,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="127">
-        <f>VLOOKUP(D24,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D24,Camere!E:Q,5,0)</f>
         <v>500</v>
       </c>
       <c r="G24">
@@ -24663,7 +24662,7 @@
         <v>19</v>
       </c>
       <c r="M24" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>31500</v>
       </c>
       <c r="N24" s="4"/>
@@ -24707,7 +24706,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="127">
-        <f>VLOOKUP(D25,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D25,Camere!E:Q,5,0)</f>
         <v>465</v>
       </c>
       <c r="G25">
@@ -24729,7 +24728,7 @@
         <v>17</v>
       </c>
       <c r="M25" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>28365</v>
       </c>
       <c r="N25" s="4"/>
@@ -24773,7 +24772,7 @@
         <v>2</v>
       </c>
       <c r="F26" s="127">
-        <f>VLOOKUP(D26,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D26,Camere!E:Q,5,0)</f>
         <v>500</v>
       </c>
       <c r="G26">
@@ -24795,7 +24794,7 @@
         <v>23</v>
       </c>
       <c r="M26" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>34000</v>
       </c>
       <c r="N26" s="4"/>
@@ -24839,7 +24838,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="129">
-        <f>VLOOKUP(D27,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D27,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G27">
@@ -24861,7 +24860,7 @@
         <v>21</v>
       </c>
       <c r="M27" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>43155</v>
       </c>
       <c r="N27" s="4"/>
@@ -24905,7 +24904,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="129">
-        <f>VLOOKUP(D28,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D28,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G28">
@@ -24927,7 +24926,7 @@
         <v>14</v>
       </c>
       <c r="M28" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>39730</v>
       </c>
       <c r="N28" s="4"/>
@@ -24971,7 +24970,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="129">
-        <f>VLOOKUP(D29,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D29,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G29">
@@ -24993,7 +24992,7 @@
         <v>16</v>
       </c>
       <c r="M29" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>40415</v>
       </c>
       <c r="N29" s="4"/>
@@ -25037,7 +25036,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="129">
-        <f>VLOOKUP(D30,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D30,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G30">
@@ -25059,7 +25058,7 @@
         <v>15</v>
       </c>
       <c r="M30" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>42470</v>
       </c>
       <c r="N30" s="4"/>
@@ -25103,7 +25102,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="129">
-        <f>VLOOKUP(D31,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D31,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G31">
@@ -25125,7 +25124,7 @@
         <v>14</v>
       </c>
       <c r="M31" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>43155</v>
       </c>
       <c r="N31" s="4"/>
@@ -25169,7 +25168,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="129">
-        <f>VLOOKUP(D32,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D32,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G32">
@@ -25191,7 +25190,7 @@
         <v>18</v>
       </c>
       <c r="M32" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>45895</v>
       </c>
       <c r="N32" s="4"/>
@@ -25235,7 +25234,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="129">
-        <f>VLOOKUP(D33,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D33,Camere!E:Q,5,0)</f>
         <v>700</v>
       </c>
       <c r="G33">
@@ -25257,7 +25256,7 @@
         <v>19</v>
       </c>
       <c r="M33" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>48300</v>
       </c>
       <c r="N33" s="4"/>
@@ -25301,7 +25300,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="129">
-        <f>VLOOKUP(D34,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D34,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G34">
@@ -25323,7 +25322,7 @@
         <v>20</v>
       </c>
       <c r="M34" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>47950</v>
       </c>
       <c r="N34" s="4"/>
@@ -25367,7 +25366,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="129">
-        <f>VLOOKUP(D35,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D35,Camere!E:Q,5,0)</f>
         <v>700</v>
       </c>
       <c r="G35">
@@ -25389,7 +25388,7 @@
         <v>18</v>
       </c>
       <c r="M35" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>43400</v>
       </c>
       <c r="N35" s="4"/>
@@ -25433,7 +25432,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="129">
-        <f>VLOOKUP(D36,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D36,Camere!E:Q,5,0)</f>
         <v>685</v>
       </c>
       <c r="G36">
@@ -25455,7 +25454,7 @@
         <v>19</v>
       </c>
       <c r="M36" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>44525</v>
       </c>
       <c r="N36" s="4"/>
@@ -25499,7 +25498,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="129">
-        <f>VLOOKUP(D37,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D37,Camere!E:Q,5,0)</f>
         <v>700</v>
       </c>
       <c r="G37">
@@ -25521,7 +25520,7 @@
         <v>16</v>
       </c>
       <c r="M37" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>41300</v>
       </c>
       <c r="N37" s="4"/>
@@ -25565,7 +25564,7 @@
         <v>138</v>
       </c>
       <c r="F38" s="125">
-        <f>VLOOKUP(D38,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D38,Camere!E:Q,5,0)</f>
         <v>845</v>
       </c>
       <c r="G38">
@@ -25587,7 +25586,7 @@
         <v>25</v>
       </c>
       <c r="M38" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>61685</v>
       </c>
       <c r="N38" s="4"/>
@@ -25631,7 +25630,7 @@
         <v>138</v>
       </c>
       <c r="F39" s="125">
-        <f>VLOOKUP(D39,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D39,Camere!E:Q,5,0)</f>
         <v>845</v>
       </c>
       <c r="G39">
@@ -25653,7 +25652,7 @@
         <v>24</v>
       </c>
       <c r="M39" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>59150</v>
       </c>
       <c r="N39" s="4"/>
@@ -25697,7 +25696,7 @@
         <v>138</v>
       </c>
       <c r="F40" s="125">
-        <f>VLOOKUP(D40,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D40,Camere!E:Q,5,0)</f>
         <v>945</v>
       </c>
       <c r="G40">
@@ -25719,7 +25718,7 @@
         <v>17</v>
       </c>
       <c r="M40" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>59535</v>
       </c>
       <c r="N40" s="4"/>
@@ -25763,7 +25762,7 @@
         <v>138</v>
       </c>
       <c r="F41" s="125">
-        <f>VLOOKUP(D41,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D41,Camere!E:Q,5,0)</f>
         <v>945</v>
       </c>
       <c r="G41">
@@ -25785,7 +25784,7 @@
         <v>17</v>
       </c>
       <c r="M41" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>56700</v>
       </c>
       <c r="N41" s="4"/>
@@ -25829,7 +25828,7 @@
         <v>138</v>
       </c>
       <c r="F42" s="125">
-        <f>VLOOKUP(D42,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D42,Camere!E:Q,5,0)</f>
         <v>945</v>
       </c>
       <c r="G42">
@@ -25851,7 +25850,7 @@
         <v>18</v>
       </c>
       <c r="M42" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>59535</v>
       </c>
       <c r="N42" s="4"/>
@@ -25895,7 +25894,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="127">
-        <f>VLOOKUP(D43,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D43,Camere!E:Q,5,0)</f>
         <v>1100</v>
       </c>
       <c r="G43">
@@ -25917,7 +25916,7 @@
         <v>19</v>
       </c>
       <c r="M43" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>67100</v>
       </c>
       <c r="N43" s="4"/>
@@ -25961,7 +25960,7 @@
         <v>5</v>
       </c>
       <c r="F44" s="127">
-        <f>VLOOKUP(D44,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D44,Camere!E:Q,5,0)</f>
         <v>1100</v>
       </c>
       <c r="G44">
@@ -25983,7 +25982,7 @@
         <v>20</v>
       </c>
       <c r="M44" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>72600</v>
       </c>
       <c r="N44" s="4"/>
@@ -26027,7 +26026,7 @@
         <v>5</v>
       </c>
       <c r="F45" s="127">
-        <f>VLOOKUP(D45,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D45,Camere!E:Q,5,0)</f>
         <v>1100</v>
       </c>
       <c r="G45">
@@ -26049,7 +26048,7 @@
         <v>19</v>
       </c>
       <c r="M45" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>69300</v>
       </c>
       <c r="N45" s="4"/>
@@ -26093,7 +26092,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="127">
-        <f>VLOOKUP(D46,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D46,Camere!E:Q,5,0)</f>
         <v>1100</v>
       </c>
       <c r="G46">
@@ -26115,7 +26114,7 @@
         <v>18</v>
       </c>
       <c r="M46" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>70400</v>
       </c>
       <c r="N46" s="4"/>
@@ -26159,7 +26158,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="127">
-        <f>VLOOKUP(D47,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D47,Camere!E:Q,5,0)</f>
         <v>1100</v>
       </c>
       <c r="G47">
@@ -26181,7 +26180,7 @@
         <v>16</v>
       </c>
       <c r="M47" s="127">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>68200</v>
       </c>
       <c r="N47" s="4"/>
@@ -26225,7 +26224,7 @@
         <v>3</v>
       </c>
       <c r="F48" s="129">
-        <f>VLOOKUP(D48,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D48,Camere!E:Q,5,0)</f>
         <v>1645</v>
       </c>
       <c r="G48">
@@ -26247,7 +26246,7 @@
         <v>19</v>
       </c>
       <c r="M48" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>98700</v>
       </c>
       <c r="N48" s="4"/>
@@ -26291,7 +26290,7 @@
         <v>3</v>
       </c>
       <c r="F49" s="129">
-        <f>VLOOKUP(D49,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D49,Camere!E:Q,5,0)</f>
         <v>1645</v>
       </c>
       <c r="G49">
@@ -26313,7 +26312,7 @@
         <v>18</v>
       </c>
       <c r="M49" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>92120</v>
       </c>
       <c r="N49" s="4"/>
@@ -26357,7 +26356,7 @@
         <v>3</v>
       </c>
       <c r="F50" s="129">
-        <f>VLOOKUP(D50,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D50,Camere!E:Q,5,0)</f>
         <v>1645</v>
       </c>
       <c r="G50">
@@ -26379,7 +26378,7 @@
         <v>17</v>
       </c>
       <c r="M50" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>92120</v>
       </c>
       <c r="N50" s="4"/>
@@ -26423,7 +26422,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="129">
-        <f>VLOOKUP(D51,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D51,Camere!E:Q,5,0)</f>
         <v>1645</v>
       </c>
       <c r="G51">
@@ -26445,7 +26444,7 @@
         <v>19</v>
       </c>
       <c r="M51" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>98700</v>
       </c>
       <c r="N51" s="4"/>
@@ -26489,7 +26488,7 @@
         <v>3</v>
       </c>
       <c r="F52" s="129">
-        <f>VLOOKUP(D52,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D52,Camere!E:Q,5,0)</f>
         <v>1645</v>
       </c>
       <c r="G52">
@@ -26511,7 +26510,7 @@
         <v>17</v>
       </c>
       <c r="M52" s="129">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>90475</v>
       </c>
       <c r="N52" s="4"/>
@@ -26555,7 +26554,7 @@
         <v>6</v>
       </c>
       <c r="F53" s="125">
-        <f>VLOOKUP(D53,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D53,Camere!E:Q,5,0)</f>
         <v>6545</v>
       </c>
       <c r="G53">
@@ -26577,7 +26576,7 @@
         <v>5</v>
       </c>
       <c r="M53" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>104720</v>
       </c>
       <c r="N53" s="4"/>
@@ -26621,7 +26620,7 @@
         <v>6</v>
       </c>
       <c r="F54" s="125">
-        <f>VLOOKUP(D54,Vehicule!E:Q,5,0)</f>
+        <f>VLOOKUP(D54,Camere!E:Q,5,0)</f>
         <v>6545</v>
       </c>
       <c r="G54">
@@ -26643,7 +26642,7 @@
         <v>7</v>
       </c>
       <c r="M54" s="125">
-        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[TARIF/KM]]</f>
+        <f>SUM(Table6[[#This Row],[IANUARIE]:[IUNIE]])*Table6[[#This Row],[PREȚ/NOAPTE]]</f>
         <v>124355</v>
       </c>
       <c r="N54" s="4"/>
@@ -29822,7 +29821,7 @@
       <c r="C41" s="4"/>
       <c r="D41" s="213" t="str">
         <f t="shared" ref="D41:L43" si="0">HLOOKUP(D5,D5:L11,5,0)</f>
-        <v>Trailer</v>
+        <v>Suită Palais</v>
       </c>
       <c r="E41" s="213">
         <f t="shared" si="0"/>
@@ -29887,7 +29886,7 @@
       <c r="C42" s="4"/>
       <c r="D42" s="213" t="str">
         <f t="shared" si="0"/>
-        <v>Autoutilitara</v>
+        <v>Suită Superioară</v>
       </c>
       <c r="E42" s="213">
         <f t="shared" si="0"/>
@@ -29952,7 +29951,7 @@
       <c r="C43" s="4"/>
       <c r="D43" s="213" t="str">
         <f t="shared" si="0"/>
-        <v>Platforma</v>
+        <v>Villa</v>
       </c>
       <c r="E43" s="213">
         <f t="shared" si="0"/>
@@ -35951,15 +35950,15 @@
         <v>203</v>
       </c>
       <c r="G5" s="168" t="str">
-        <f>VLOOKUP(F5,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F5,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H5" s="170">
-        <f>VLOOKUP(F5,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F5,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I5" s="170">
-        <f>VLOOKUP(F5,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F5,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J5" s="168">
@@ -36012,15 +36011,15 @@
         <v>205</v>
       </c>
       <c r="G6" s="168" t="str">
-        <f>VLOOKUP(F6,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F6,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H6" s="170">
-        <f>VLOOKUP(F6,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F6,Camere!E:N,9,0)</f>
         <v>43665</v>
       </c>
       <c r="I6" s="170">
-        <f>VLOOKUP(F6,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F6,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J6" s="168">
@@ -36073,15 +36072,15 @@
         <v>301</v>
       </c>
       <c r="G7" s="168" t="str">
-        <f>VLOOKUP(F7,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F7,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H7" s="170">
-        <f>VLOOKUP(F7,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F7,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I7" s="170">
-        <f>VLOOKUP(F7,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F7,Camere!E:N,10,0)</f>
         <v>47325</v>
       </c>
       <c r="J7" s="168">
@@ -36134,15 +36133,15 @@
         <v>305</v>
       </c>
       <c r="G8" s="168" t="str">
-        <f>VLOOKUP(F8,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F8,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H8" s="170">
-        <f>VLOOKUP(F8,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F8,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I8" s="170">
-        <f>VLOOKUP(F8,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F8,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J8" s="168">
@@ -36195,15 +36194,15 @@
         <v>401</v>
       </c>
       <c r="G9" s="168" t="str">
-        <f>VLOOKUP(F9,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F9,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H9" s="170">
-        <f>VLOOKUP(F9,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F9,Camere!E:N,9,0)</f>
         <v>43671</v>
       </c>
       <c r="I9" s="170">
-        <f>VLOOKUP(F9,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F9,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J9" s="168">
@@ -36256,15 +36255,15 @@
         <v>403</v>
       </c>
       <c r="G10" s="168" t="str">
-        <f>VLOOKUP(F10,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F10,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H10" s="170">
-        <f>VLOOKUP(F10,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F10,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I10" s="170">
-        <f>VLOOKUP(F10,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F10,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J10" s="168">
@@ -36317,15 +36316,15 @@
         <v>501</v>
       </c>
       <c r="G11" s="168" t="str">
-        <f>VLOOKUP(F11,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F11,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H11" s="170">
-        <f>VLOOKUP(F11,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F11,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I11" s="170">
-        <f>VLOOKUP(F11,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F11,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J11" s="168">
@@ -36378,15 +36377,15 @@
         <v>503</v>
       </c>
       <c r="G12" s="168" t="str">
-        <f>VLOOKUP(F12,Curse_S1!D:M,2,0)</f>
-        <v>Camion</v>
+        <f>VLOOKUP(F12,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Superioară</v>
       </c>
       <c r="H12" s="170">
-        <f>VLOOKUP(F12,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F12,Camere!E:N,9,0)</f>
         <v>43666</v>
       </c>
       <c r="I12" s="170">
-        <f>VLOOKUP(F12,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F12,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J12" s="168">
@@ -36439,15 +36438,15 @@
         <v>202</v>
       </c>
       <c r="G13" s="168" t="str">
-        <f>VLOOKUP(F13,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F13,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H13" s="170">
-        <f>VLOOKUP(F13,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F13,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I13" s="170">
-        <f>VLOOKUP(F13,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F13,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J13" s="168">
@@ -36500,15 +36499,15 @@
         <v>204</v>
       </c>
       <c r="G14" s="168" t="str">
-        <f>VLOOKUP(F14,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F14,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H14" s="170">
-        <f>VLOOKUP(F14,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F14,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I14" s="170">
-        <f>VLOOKUP(F14,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F14,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J14" s="168">
@@ -36561,15 +36560,15 @@
         <v>302</v>
       </c>
       <c r="G15" s="168" t="str">
-        <f>VLOOKUP(F15,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F15,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H15" s="170">
-        <f>VLOOKUP(F15,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F15,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I15" s="170">
-        <f>VLOOKUP(F15,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F15,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J15" s="168">
@@ -36622,15 +36621,15 @@
         <v>304</v>
       </c>
       <c r="G16" s="168" t="str">
-        <f>VLOOKUP(F16,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F16,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H16" s="170">
-        <f>VLOOKUP(F16,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F16,Camere!E:N,9,0)</f>
         <v>43667</v>
       </c>
       <c r="I16" s="170">
-        <f>VLOOKUP(F16,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F16,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J16" s="168">
@@ -36683,15 +36682,15 @@
         <v>402</v>
       </c>
       <c r="G17" s="168" t="str">
-        <f>VLOOKUP(F17,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F17,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H17" s="170">
-        <f>VLOOKUP(F17,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F17,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I17" s="170">
-        <f>VLOOKUP(F17,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F17,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J17" s="168">
@@ -36744,15 +36743,15 @@
         <v>404</v>
       </c>
       <c r="G18" s="168" t="str">
-        <f>VLOOKUP(F18,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F18,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H18" s="170">
-        <f>VLOOKUP(F18,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F18,Camere!E:N,9,0)</f>
         <v>43671</v>
       </c>
       <c r="I18" s="170">
-        <f>VLOOKUP(F18,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F18,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J18" s="168">
@@ -36805,15 +36804,15 @@
         <v>406</v>
       </c>
       <c r="G19" s="168" t="str">
-        <f>VLOOKUP(F19,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F19,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H19" s="170">
-        <f>VLOOKUP(F19,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F19,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I19" s="170">
-        <f>VLOOKUP(F19,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F19,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J19" s="168">
@@ -36866,15 +36865,15 @@
         <v>504</v>
       </c>
       <c r="G20" s="168" t="str">
-        <f>VLOOKUP(F20,Curse_S1!D:M,2,0)</f>
-        <v>Duba</v>
+        <f>VLOOKUP(F20,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Delux</v>
       </c>
       <c r="H20" s="170">
-        <f>VLOOKUP(F20,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F20,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I20" s="170">
-        <f>VLOOKUP(F20,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F20,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J20" s="168">
@@ -36927,15 +36926,15 @@
         <v>207</v>
       </c>
       <c r="G21" s="168" t="str">
-        <f>VLOOKUP(F21,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F21,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H21" s="170">
-        <f>VLOOKUP(F21,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F21,Camere!E:N,9,0)</f>
         <v>43667</v>
       </c>
       <c r="I21" s="170">
-        <f>VLOOKUP(F21,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F21,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J21" s="168">
@@ -36988,15 +36987,15 @@
         <v>208</v>
       </c>
       <c r="G22" s="168" t="str">
-        <f>VLOOKUP(F22,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F22,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H22" s="170">
-        <f>VLOOKUP(F22,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F22,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I22" s="170">
-        <f>VLOOKUP(F22,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F22,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J22" s="168">
@@ -37049,15 +37048,15 @@
         <v>209</v>
       </c>
       <c r="G23" s="168" t="str">
-        <f>VLOOKUP(F23,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F23,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H23" s="170">
-        <f>VLOOKUP(F23,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F23,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I23" s="170">
-        <f>VLOOKUP(F23,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F23,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J23" s="168">
@@ -37110,15 +37109,15 @@
         <v>307</v>
       </c>
       <c r="G24" s="168" t="str">
-        <f>VLOOKUP(F24,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F24,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H24" s="170">
-        <f>VLOOKUP(F24,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F24,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I24" s="170">
-        <f>VLOOKUP(F24,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F24,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J24" s="168">
@@ -37171,15 +37170,15 @@
         <v>308</v>
       </c>
       <c r="G25" s="168" t="str">
-        <f>VLOOKUP(F25,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F25,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H25" s="170">
-        <f>VLOOKUP(F25,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F25,Camere!E:N,9,0)</f>
         <v>43665</v>
       </c>
       <c r="I25" s="170">
-        <f>VLOOKUP(F25,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F25,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J25" s="168">
@@ -37232,15 +37231,15 @@
         <v>407</v>
       </c>
       <c r="G26" s="168" t="str">
-        <f>VLOOKUP(F26,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F26,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H26" s="170">
-        <f>VLOOKUP(F26,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F26,Camere!E:N,9,0)</f>
         <v>43666</v>
       </c>
       <c r="I26" s="170">
-        <f>VLOOKUP(F26,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F26,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J26" s="168">
@@ -37293,15 +37292,15 @@
         <v>408</v>
       </c>
       <c r="G27" s="168" t="str">
-        <f>VLOOKUP(F27,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F27,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H27" s="170">
-        <f>VLOOKUP(F27,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F27,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I27" s="170">
-        <f>VLOOKUP(F27,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F27,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J27" s="168">
@@ -37354,15 +37353,15 @@
         <v>409</v>
       </c>
       <c r="G28" s="168" t="str">
-        <f>VLOOKUP(F28,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F28,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H28" s="170">
-        <f>VLOOKUP(F28,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F28,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I28" s="170">
-        <f>VLOOKUP(F28,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F28,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J28" s="168">
@@ -37415,15 +37414,15 @@
         <v>507</v>
       </c>
       <c r="G29" s="168" t="str">
-        <f>VLOOKUP(F29,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F29,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H29" s="170">
-        <f>VLOOKUP(F29,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F29,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I29" s="170">
-        <f>VLOOKUP(F29,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F29,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J29" s="168">
@@ -37476,15 +37475,15 @@
         <v>508</v>
       </c>
       <c r="G30" s="168" t="str">
-        <f>VLOOKUP(F30,Curse_S1!D:M,2,0)</f>
-        <v>Autocar</v>
+        <f>VLOOKUP(F30,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Cameră Palais</v>
       </c>
       <c r="H30" s="170">
-        <f>VLOOKUP(F30,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F30,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I30" s="170">
-        <f>VLOOKUP(F30,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F30,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J30" s="168">
@@ -37537,15 +37536,15 @@
         <v>310</v>
       </c>
       <c r="G31" s="168" t="str">
-        <f>VLOOKUP(F31,Curse_S1!D:M,2,0)</f>
-        <v>Autoutilitara</v>
+        <f>VLOOKUP(F31,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Superioară</v>
       </c>
       <c r="H31" s="170">
-        <f>VLOOKUP(F31,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F31,Camere!E:N,9,0)</f>
         <v>43667</v>
       </c>
       <c r="I31" s="170">
-        <f>VLOOKUP(F31,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F31,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J31" s="168">
@@ -37598,15 +37597,15 @@
         <v>410</v>
       </c>
       <c r="G32" s="168" t="str">
-        <f>VLOOKUP(F32,Curse_S1!D:M,2,0)</f>
-        <v>Autoutilitara</v>
+        <f>VLOOKUP(F32,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Superioară</v>
       </c>
       <c r="H32" s="170">
-        <f>VLOOKUP(F32,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F32,Camere!E:N,9,0)</f>
         <v>43671</v>
       </c>
       <c r="I32" s="170">
-        <f>VLOOKUP(F32,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F32,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J32" s="168">
@@ -37659,15 +37658,15 @@
         <v>510</v>
       </c>
       <c r="G33" s="168" t="str">
-        <f>VLOOKUP(F33,Curse_S1!D:M,2,0)</f>
-        <v>Autoutilitara</v>
+        <f>VLOOKUP(F33,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Superioară</v>
       </c>
       <c r="H33" s="170">
-        <f>VLOOKUP(F33,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F33,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I33" s="170">
-        <f>VLOOKUP(F33,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F33,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J33" s="168">
@@ -37720,15 +37719,15 @@
         <v>411</v>
       </c>
       <c r="G34" s="168" t="str">
-        <f>VLOOKUP(F34,Curse_S1!D:M,2,0)</f>
-        <v>Semiremorca</v>
+        <f>VLOOKUP(F34,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Delux</v>
       </c>
       <c r="H34" s="170">
-        <f>VLOOKUP(F34,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F34,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I34" s="170">
-        <f>VLOOKUP(F34,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F34,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J34" s="168">
@@ -37781,15 +37780,15 @@
         <v>412</v>
       </c>
       <c r="G35" s="168" t="str">
-        <f>VLOOKUP(F35,Curse_S1!D:M,2,0)</f>
-        <v>Semiremorca</v>
+        <f>VLOOKUP(F35,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Delux</v>
       </c>
       <c r="H35" s="170">
-        <f>VLOOKUP(F35,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F35,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I35" s="170">
-        <f>VLOOKUP(F35,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F35,Camere!E:N,10,0)</f>
         <v>43671</v>
       </c>
       <c r="J35" s="168">
@@ -37842,15 +37841,15 @@
         <v>513</v>
       </c>
       <c r="G36" s="168" t="str">
-        <f>VLOOKUP(F36,Curse_S1!D:M,2,0)</f>
-        <v>Semiremorca</v>
+        <f>VLOOKUP(F36,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Delux</v>
       </c>
       <c r="H36" s="170">
-        <f>VLOOKUP(F36,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F36,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I36" s="170">
-        <f>VLOOKUP(F36,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F36,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J36" s="168">
@@ -37903,15 +37902,15 @@
         <v>104</v>
       </c>
       <c r="G37" s="168" t="str">
-        <f>VLOOKUP(F37,Curse_S1!D:M,2,0)</f>
-        <v>Semiremorca</v>
+        <f>VLOOKUP(F37,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Delux</v>
       </c>
       <c r="H37" s="170">
-        <f>VLOOKUP(F37,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F37,Camere!E:N,9,0)</f>
         <v>43670</v>
       </c>
       <c r="I37" s="170">
-        <f>VLOOKUP(F37,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F37,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J37" s="168">
@@ -37964,15 +37963,15 @@
         <v>101</v>
       </c>
       <c r="G38" s="168" t="str">
-        <f>VLOOKUP(F38,Curse_S1!D:M,2,0)</f>
-        <v>Trailer</v>
+        <f>VLOOKUP(F38,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Palais</v>
       </c>
       <c r="H38" s="170">
-        <f>VLOOKUP(F38,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F38,Camere!E:N,9,0)</f>
         <v>43667</v>
       </c>
       <c r="I38" s="170">
-        <f>VLOOKUP(F38,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F38,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J38" s="168">
@@ -38025,15 +38024,15 @@
         <v>102</v>
       </c>
       <c r="G39" s="168" t="str">
-        <f>VLOOKUP(F39,Curse_S1!D:M,2,0)</f>
-        <v>Trailer</v>
+        <f>VLOOKUP(F39,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Palais</v>
       </c>
       <c r="H39" s="170">
-        <f>VLOOKUP(F39,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F39,Camere!E:N,9,0)</f>
         <v>43668</v>
       </c>
       <c r="I39" s="170">
-        <f>VLOOKUP(F39,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F39,Camere!E:N,10,0)</f>
         <v>43672</v>
       </c>
       <c r="J39" s="168">
@@ -38086,15 +38085,15 @@
         <v>602</v>
       </c>
       <c r="G40" s="168" t="str">
-        <f>VLOOKUP(F40,Curse_S1!D:M,2,0)</f>
-        <v>Trailer</v>
+        <f>VLOOKUP(F40,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Palais</v>
       </c>
       <c r="H40" s="170">
-        <f>VLOOKUP(F40,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F40,Camere!E:N,9,0)</f>
         <v>43671</v>
       </c>
       <c r="I40" s="170">
-        <f>VLOOKUP(F40,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F40,Camere!E:N,10,0)</f>
         <v>43674</v>
       </c>
       <c r="J40" s="168">
@@ -38147,15 +38146,15 @@
         <v>603</v>
       </c>
       <c r="G41" s="168" t="str">
-        <f>VLOOKUP(F41,Curse_S1!D:M,2,0)</f>
-        <v>Trailer</v>
+        <f>VLOOKUP(F41,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Suită Palais</v>
       </c>
       <c r="H41" s="170">
-        <f>VLOOKUP(F41,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F41,Camere!E:N,9,0)</f>
         <v>43669</v>
       </c>
       <c r="I41" s="170">
-        <f>VLOOKUP(F41,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F41,Camere!E:N,10,0)</f>
         <v>43675</v>
       </c>
       <c r="J41" s="168">
@@ -38208,15 +38207,15 @@
         <v>1</v>
       </c>
       <c r="G42" s="174" t="str">
-        <f>VLOOKUP(F42,Curse_S1!D:M,2,0)</f>
-        <v>Platforma</v>
+        <f>VLOOKUP(F42,'Nr nopți ocpt in prima jum an'!D:M,2,0)</f>
+        <v>Villa</v>
       </c>
       <c r="H42" s="176">
-        <f>VLOOKUP(F42,Vehicule!E:N,9,0)</f>
+        <f>VLOOKUP(F42,Camere!E:N,9,0)</f>
         <v>43667</v>
       </c>
       <c r="I42" s="176">
-        <f>VLOOKUP(F42,Vehicule!E:N,10,0)</f>
+        <f>VLOOKUP(F42,Camere!E:N,10,0)</f>
         <v>43673</v>
       </c>
       <c r="J42" s="174">

</xml_diff>